<commit_message>
--CuongDVT-- Bổ sung chú thích cho chức năng rút tiền
</commit_message>
<xml_diff>
--- a/Documents/Model/DetailsFnc.xlsx
+++ b/Documents/Model/DetailsFnc.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phuc\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SVN - GoogleCode\atm-web-demo\Documents\Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="132">
   <si>
     <t>Class</t>
   </si>
@@ -351,6 +351,75 @@
   </si>
   <si>
     <t>.</t>
+  </si>
+  <si>
+    <t>ACCOUNT</t>
+  </si>
+  <si>
+    <t>AcountID</t>
+  </si>
+  <si>
+    <t>ID tài khoản</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>Sô dư tài khoản</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Thông tin khách hàng</t>
+  </si>
+  <si>
+    <t>Kiểm tra số tiền rút</t>
+  </si>
+  <si>
+    <t>CASH DISPENSER</t>
+  </si>
+  <si>
+    <t>DispenseCash(ATM inATM)</t>
+  </si>
+  <si>
+    <t>CheckWithdrawCash(float inWithdrawAmout)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trả tiền </t>
+  </si>
+  <si>
+    <t>STOCK</t>
+  </si>
+  <si>
+    <t>MoneyID</t>
+  </si>
+  <si>
+    <t>GetAllMoney(int inMoneyID)</t>
+  </si>
+  <si>
+    <t>Money</t>
+  </si>
+  <si>
+    <t>StookID</t>
+  </si>
+  <si>
+    <t>ID kho lưu trữ</t>
+  </si>
+  <si>
+    <t>ID tiền</t>
+  </si>
+  <si>
+    <t>ID ATM</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>số lượng</t>
+  </si>
+  <si>
+    <t>Xem tất cả các loại tiền</t>
   </si>
 </sst>
 </file>
@@ -392,7 +461,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -452,11 +521,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -477,34 +588,49 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -787,21 +913,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:H54"/>
+  <dimension ref="B5:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E29" workbookViewId="0">
-      <selection activeCell="G51" sqref="B5:G51"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="7"/>
-    <col min="2" max="2" width="17.85546875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="14"/>
-    <col min="5" max="5" width="27.5703125" style="15" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" style="17" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="11"/>
+    <col min="5" max="5" width="27.5703125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" style="14" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
@@ -825,8 +951,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
+    <row r="6" spans="2:7" ht="63" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="2"/>
@@ -839,12 +965,12 @@
       <c r="F6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="10"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="2"/>
       <c r="D7" s="3" t="s">
         <v>6</v>
@@ -855,12 +981,12 @@
       <c r="F7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="10"/>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="16"/>
       <c r="C8" s="2"/>
       <c r="D8" s="3" t="s">
         <v>6</v>
@@ -871,12 +997,12 @@
       <c r="F8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="10"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="2"/>
       <c r="D9" s="3" t="s">
         <v>6</v>
@@ -887,12 +1013,12 @@
       <c r="F9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B10" s="10"/>
+    <row r="10" spans="2:7" ht="63" x14ac:dyDescent="0.25">
+      <c r="B10" s="16"/>
       <c r="C10" s="2"/>
       <c r="D10" s="3" t="s">
         <v>6</v>
@@ -903,12 +1029,12 @@
       <c r="F10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="63" x14ac:dyDescent="0.25">
-      <c r="B11" s="10"/>
+    <row r="11" spans="2:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B11" s="16"/>
       <c r="C11" s="2"/>
       <c r="D11" s="3" t="s">
         <v>6</v>
@@ -919,12 +1045,12 @@
       <c r="F11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="10"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
@@ -935,12 +1061,12 @@
       <c r="F12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="10"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
@@ -951,12 +1077,12 @@
       <c r="F13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B14" s="10"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="2" t="s">
         <v>6</v>
       </c>
@@ -967,12 +1093,12 @@
       <c r="F14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B15" s="11"/>
+    <row r="15" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B15" s="17"/>
       <c r="C15" s="2" t="s">
         <v>6</v>
       </c>
@@ -983,12 +1109,12 @@
       <c r="F15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="2"/>
@@ -1001,12 +1127,12 @@
       <c r="F16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="10"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="2"/>
       <c r="D17" s="3" t="s">
         <v>6</v>
@@ -1017,12 +1143,12 @@
       <c r="F17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="10"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="2"/>
       <c r="D18" s="3" t="s">
         <v>6</v>
@@ -1033,12 +1159,12 @@
       <c r="F18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G18" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="10"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="2"/>
       <c r="D19" s="3" t="s">
         <v>6</v>
@@ -1049,12 +1175,12 @@
       <c r="F19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" s="8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="11"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="2" t="s">
         <v>6</v>
       </c>
@@ -1065,12 +1191,12 @@
       <c r="F20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="15" t="s">
         <v>44</v>
       </c>
       <c r="C21" s="2"/>
@@ -1083,12 +1209,12 @@
       <c r="F21" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="G21" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="10"/>
+      <c r="B22" s="16"/>
       <c r="C22" s="2"/>
       <c r="D22" s="3" t="s">
         <v>6</v>
@@ -1099,12 +1225,12 @@
       <c r="F22" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="G22" s="8" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="10"/>
+      <c r="B23" s="16"/>
       <c r="C23" s="2"/>
       <c r="D23" s="3" t="s">
         <v>6</v>
@@ -1115,12 +1241,12 @@
       <c r="F23" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="G23" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="10"/>
+      <c r="B24" s="16"/>
       <c r="C24" s="2"/>
       <c r="D24" s="3" t="s">
         <v>6</v>
@@ -1131,12 +1257,12 @@
       <c r="F24" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="G24" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="10"/>
+      <c r="B25" s="16"/>
       <c r="C25" s="2"/>
       <c r="D25" s="3" t="s">
         <v>6</v>
@@ -1147,12 +1273,12 @@
       <c r="F25" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="G25" s="8" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="10"/>
+      <c r="B26" s="16"/>
       <c r="C26" s="2" t="s">
         <v>6</v>
       </c>
@@ -1163,12 +1289,12 @@
       <c r="F26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="G26" s="8" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="10"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="2" t="s">
         <v>6</v>
       </c>
@@ -1179,12 +1305,12 @@
       <c r="F27" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G27" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B28" s="10"/>
+    <row r="28" spans="2:7" ht="63" x14ac:dyDescent="0.25">
+      <c r="B28" s="16"/>
       <c r="C28" s="2" t="s">
         <v>6</v>
       </c>
@@ -1195,12 +1321,12 @@
       <c r="F28" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="G28" s="8" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B29" s="10"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="2" t="s">
         <v>6</v>
       </c>
@@ -1211,12 +1337,12 @@
       <c r="F29" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G29" s="9" t="s">
+      <c r="G29" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="63" x14ac:dyDescent="0.25">
-      <c r="B30" s="10"/>
+    <row r="30" spans="2:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B30" s="16"/>
       <c r="C30" s="2" t="s">
         <v>6</v>
       </c>
@@ -1227,12 +1353,12 @@
       <c r="F30" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G30" s="9" t="s">
+      <c r="G30" s="8" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="11"/>
+      <c r="B31" s="17"/>
       <c r="C31" s="2" t="s">
         <v>6</v>
       </c>
@@ -1243,12 +1369,12 @@
       <c r="F31" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G31" s="9" t="s">
+      <c r="G31" s="8" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="15" t="s">
         <v>67</v>
       </c>
       <c r="C32" s="2"/>
@@ -1261,12 +1387,12 @@
       <c r="F32" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G32" s="9" t="s">
+      <c r="G32" s="8" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B33" s="10"/>
+      <c r="B33" s="16"/>
       <c r="C33" s="2"/>
       <c r="D33" s="3" t="s">
         <v>6</v>
@@ -1277,12 +1403,12 @@
       <c r="F33" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G33" s="9" t="s">
+      <c r="G33" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="10"/>
+      <c r="B34" s="16"/>
       <c r="C34" s="2"/>
       <c r="D34" s="3" t="s">
         <v>6</v>
@@ -1293,12 +1419,12 @@
       <c r="F34" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G34" s="9" t="s">
+      <c r="G34" s="8" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="35" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B35" s="10"/>
+      <c r="B35" s="16"/>
       <c r="C35" s="2" t="s">
         <v>6</v>
       </c>
@@ -1309,12 +1435,12 @@
       <c r="F35" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G35" s="9" t="s">
+      <c r="G35" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B36" s="11"/>
+      <c r="B36" s="17"/>
       <c r="C36" s="2" t="s">
         <v>6</v>
       </c>
@@ -1325,12 +1451,12 @@
       <c r="F36" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G36" s="9" t="s">
+      <c r="G36" s="8" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="15" t="s">
         <v>77</v>
       </c>
       <c r="C37" s="2" t="s">
@@ -1343,12 +1469,12 @@
       <c r="F37" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G37" s="9" t="s">
+      <c r="G37" s="8" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="10"/>
+      <c r="B38" s="16"/>
       <c r="C38" s="2" t="s">
         <v>6</v>
       </c>
@@ -1359,12 +1485,12 @@
       <c r="F38" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="G38" s="9" t="s">
+      <c r="G38" s="8" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="10"/>
+      <c r="B39" s="16"/>
       <c r="C39" s="2" t="s">
         <v>6</v>
       </c>
@@ -1375,12 +1501,12 @@
       <c r="F39" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G39" s="9" t="s">
+      <c r="G39" s="8" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="11"/>
+      <c r="B40" s="17"/>
       <c r="C40" s="2" t="s">
         <v>6</v>
       </c>
@@ -1391,12 +1517,12 @@
       <c r="F40" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G40" s="9" t="s">
+      <c r="G40" s="8" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="15" t="s">
         <v>87</v>
       </c>
       <c r="C41" s="2"/>
@@ -1409,12 +1535,12 @@
       <c r="F41" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G41" s="9" t="s">
+      <c r="G41" s="8" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="10"/>
+      <c r="B42" s="16"/>
       <c r="C42" s="2"/>
       <c r="D42" s="3" t="s">
         <v>6</v>
@@ -1425,12 +1551,12 @@
       <c r="F42" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="G42" s="9" t="s">
+      <c r="G42" s="8" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="10"/>
+      <c r="B43" s="16"/>
       <c r="C43" s="2"/>
       <c r="D43" s="3" t="s">
         <v>6</v>
@@ -1441,12 +1567,12 @@
       <c r="F43" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G43" s="9" t="s">
+      <c r="G43" s="8" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="10"/>
+      <c r="B44" s="16"/>
       <c r="C44" s="2"/>
       <c r="D44" s="3" t="s">
         <v>6</v>
@@ -1457,12 +1583,12 @@
       <c r="F44" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="G44" s="9" t="s">
+      <c r="G44" s="8" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="10"/>
+      <c r="B45" s="16"/>
       <c r="C45" s="2"/>
       <c r="D45" s="3" t="s">
         <v>6</v>
@@ -1473,12 +1599,12 @@
       <c r="F45" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="G45" s="9" t="s">
+      <c r="G45" s="8" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="10"/>
+      <c r="B46" s="16"/>
       <c r="C46" s="2"/>
       <c r="D46" s="3" t="s">
         <v>6</v>
@@ -1489,12 +1615,12 @@
       <c r="F46" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G46" s="9" t="s">
+      <c r="G46" s="8" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="10"/>
+      <c r="B47" s="16"/>
       <c r="C47" s="2" t="s">
         <v>6</v>
       </c>
@@ -1505,12 +1631,12 @@
       <c r="F47" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G47" s="9" t="s">
+      <c r="G47" s="8" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="48" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B48" s="11"/>
+      <c r="B48" s="17"/>
       <c r="C48" s="2" t="s">
         <v>6</v>
       </c>
@@ -1521,12 +1647,12 @@
       <c r="F48" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="G48" s="9" t="s">
+      <c r="G48" s="8" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="15" t="s">
         <v>105</v>
       </c>
       <c r="C49" s="2"/>
@@ -1539,12 +1665,12 @@
       <c r="F49" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G49" s="9" t="s">
+      <c r="G49" s="8" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="10"/>
+      <c r="B50" s="16"/>
       <c r="C50" s="2"/>
       <c r="D50" s="3" t="s">
         <v>6</v>
@@ -1555,12 +1681,12 @@
       <c r="F50" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G50" s="9" t="s">
+      <c r="G50" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="11"/>
+      <c r="B51" s="17"/>
       <c r="C51" s="2" t="s">
         <v>6</v>
       </c>
@@ -1571,7 +1697,7 @@
       <c r="F51" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="G51" s="9" t="s">
+      <c r="G51" s="8" t="s">
         <v>98</v>
       </c>
       <c r="H51" s="7" t="s">
@@ -1579,31 +1705,175 @@
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B52" s="1"/>
+      <c r="B52" s="19" t="s">
+        <v>109</v>
+      </c>
       <c r="C52" s="2"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="9"/>
+      <c r="D52" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B53" s="1"/>
+      <c r="B53" s="20"/>
       <c r="C53" s="2"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="9"/>
+      <c r="D53" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="1"/>
+      <c r="B54" s="20"/>
       <c r="C54" s="2"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="9"/>
+      <c r="D54" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G54" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B55" s="21"/>
+      <c r="C55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="3"/>
+      <c r="E55" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G55" s="22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C56" s="2"/>
+      <c r="D56" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="3"/>
+      <c r="E57" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G57" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="18"/>
+      <c r="C58" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="3"/>
+      <c r="E58" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G58" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="18"/>
+      <c r="C59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="3"/>
+      <c r="E59" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G59" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="18"/>
+      <c r="C60" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="3"/>
+      <c r="E60" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G60" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="18"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G61" s="8" t="s">
+        <v>131</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="B57:B61"/>
     <mergeCell ref="B49:B51"/>
     <mergeCell ref="B6:B15"/>
     <mergeCell ref="B16:B20"/>

</xml_diff>